<commit_message>
Se añaden configuraciones al Config para agilizar las corridas. Se optimiza el sistema de captura de comentarios (sin respuestas).
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourseREF\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E8B568F-38F5-45DF-8D0F-BCB678482F03}"/>
   <bookViews>
-    <workbookView xWindow="10605" yWindow="2760" windowWidth="16215" windowHeight="10410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -196,7 +196,20 @@
 Son milisegundos (2mil milisegundos = 2 segundos)</t>
   </si>
   <si>
-    <t>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourseREF\Data\Output</t>
+    <t>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</t>
+  </si>
+  <si>
+    <t>DarFormatoReporte</t>
+  </si>
+  <si>
+    <t>Si deseas no dar formato (tamaño de columnas) para agilizar el resutlado, puedes cambiar esta bandera a FALSE.</t>
+  </si>
+  <si>
+    <t>ActivarModoDebug</t>
+  </si>
+  <si>
+    <t>Si el Value es TRUE solo realizará un recorrido a las 2 primeras clases que encuentre. La intención de esta bandera es agilizar la depuración.
+Si el Value es False, realizará el recorrido de todas las clases que encuentre.</t>
   </si>
 </sst>
 </file>
@@ -589,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -671,7 +684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="60">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -709,7 +722,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>47</v>
@@ -748,8 +761,35 @@
         <v>49</v>
       </c>
     </row>
+    <row r="12" spans="1:26" ht="30">
+      <c r="A12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="45">
+      <c r="A13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B13 B8:B10" xr:uid="{B289504C-077C-4D37-97DF-E19AC25F6065}">
+      <formula1>"False, True"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -822,7 +862,7 @@
       </c>
       <c r="B3" t="str">
         <f>Settings!B5</f>
-        <v>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourseREF\Data\Output</v>
+        <v>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Se añaden correcciones y controles de errores para hacer merge en el Excel cuando no hay datos en alguna de las 2 hojas.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E8B568F-38F5-45DF-8D0F-BCB678482F03}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F76BA57-BDE2-4006-9FA9-1DDCCFDFDE26}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,9 +189,6 @@
     <t>Este valor se convierte en Segundos, al colocar 1 genera que cada actividad de formato tenga un tiempo de espera de &lt;tuvalor&gt;*2 segundo. Son apróximadamente 15 actividades de Formato.</t>
   </si>
   <si>
-    <t>platzi.com/uipath</t>
-  </si>
-  <si>
     <t>Entre mayor este número más tardará el robot, recuerda 1 segundo por cada mil escrito en el valor.
 Son milisegundos (2mil milisegundos = 2 segundos)</t>
   </si>
@@ -202,14 +199,17 @@
     <t>DarFormatoReporte</t>
   </si>
   <si>
-    <t>Si deseas no dar formato (tamaño de columnas) para agilizar el resutlado, puedes cambiar esta bandera a FALSE.</t>
-  </si>
-  <si>
     <t>ActivarModoDebug</t>
   </si>
   <si>
     <t>Si el Value es TRUE solo realizará un recorrido a las 2 primeras clases que encuentre. La intención de esta bandera es agilizar la depuración.
 Si el Value es False, realizará el recorrido de todas las clases que encuentre.</t>
+  </si>
+  <si>
+    <t>Si deseas no dar formato (tamaño de columnas, añadir comentarios) para agilizar el resultado, puedes cambiar esta bandera a FALSE.</t>
+  </si>
+  <si>
+    <t>https://platzi.com/clases/uipath/</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -678,7 +678,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>30</v>
@@ -689,7 +689,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>36</v>
@@ -714,7 +714,7 @@
         <v>2000</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30">
@@ -763,24 +763,24 @@
     </row>
     <row r="12" spans="1:26" ht="30">
       <c r="A12" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="45">
       <c r="A13" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se optimiza el sistema Formato de documento, ahora crea un respaldo antes de dar formato.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F76BA57-BDE2-4006-9FA9-1DDCCFDFDE26}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3135EA0-6724-4736-996A-0D790295BF2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>https://platzi.com/clases/uipath/</t>
+  </si>
+  <si>
+    <t>Navegador</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).</t>
   </si>
 </sst>
 </file>
@@ -602,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -783,11 +792,25 @@
         <v>54</v>
       </c>
     </row>
+    <row r="14" spans="1:26" ht="30">
+      <c r="A14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B13 B8:B10" xr:uid="{B289504C-077C-4D37-97DF-E19AC25F6065}">
-      <formula1>"False, True"</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Valor inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B14" xr:uid="{D5ABB2E3-00BB-47FB-BB5C-0A9FF1640B9C}">
+      <formula1>"Firefox, Edge, Chrome, InternetExplorer"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B13 B12 B10 B8 B9" xr:uid="{128881F2-0E38-4DFD-A3D4-6EB6C88D1173}">
+      <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se actualiza y corrige el sistema de ClosePlatziCourseTab para que tenga soporte para todos los navegadores autorizados por UiPath
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3135EA0-6724-4736-996A-0D790295BF2B}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B737493-6713-48E4-9D51-557DBF443625}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,10 +215,10 @@
     <t>Navegador</t>
   </si>
   <si>
-    <t>Firefox</t>
-  </si>
-  <si>
     <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).</t>
+  </si>
+  <si>
+    <t>InternetExplorer</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -797,10 +797,10 @@
         <v>57</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añade soporte para todos los navegadores que soporta UiPath.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B737493-6713-48E4-9D51-557DBF443625}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FBE7A52-F6BD-44A5-A5B9-7E499C3D8C68}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,7 +218,7 @@
     <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).</t>
   </si>
   <si>
-    <t>InternetExplorer</t>
+    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Se añade soporte de multi browser en seguimiento automático y manual. Se añade sistema para cerrar reporte antes de leerlo por si está abierto. Se extrae funcionalidad repetida a xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{36CA22D4-D722-4A73-85D4-D3A75A56C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FBE7A52-F6BD-44A5-A5B9-7E499C3D8C68}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C719AB-BA20-47F3-A280-4DF756DAE073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30675" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -123,102 +123,100 @@
   </si>
   <si>
     <t>PlatziCourse</t>
+  </si>
+  <si>
+    <t>URLCursos</t>
+  </si>
+  <si>
+    <t>RutaPadre</t>
+  </si>
+  <si>
+    <t>NombreReporte</t>
+  </si>
+  <si>
+    <t>Comentarios.xlsx</t>
+  </si>
+  <si>
+    <t>Nombre que se le asignará al archivo excel del reporte final.</t>
+  </si>
+  <si>
+    <t>Ruta donde se guardará el archivo final, capturas de pantalla y logs.</t>
+  </si>
+  <si>
+    <t>LogLocal</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>True: generará un log llamadlo log.txt en la ruta padre.
+False: No generará ningún reporte.</t>
+  </si>
+  <si>
+    <t>varTimeOutGeneral</t>
+  </si>
+  <si>
+    <t>ExtraerRespuestasDeComentarios</t>
+  </si>
+  <si>
+    <t>SeguimientoManual</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>SeguimientoAutomático</t>
+  </si>
+  <si>
+    <t>Volverá el robot un robot Atendido y solicitará respuesta para cada comentario encontrado.</t>
+  </si>
+  <si>
+    <t>Responderá automáticamente a cada comentario que cumpla las condiciones de respuesta automática</t>
+  </si>
+  <si>
+    <t>Indica si deseas o no extraer las respuestas de cada comentario.</t>
+  </si>
+  <si>
+    <t>delayGenerarReporte</t>
+  </si>
+  <si>
+    <t>Este valor se convierte en Segundos, al colocar 1 genera que cada actividad de formato tenga un tiempo de espera de &lt;tuvalor&gt;*2 segundo. Son apróximadamente 15 actividades de Formato.</t>
+  </si>
+  <si>
+    <t>Entre mayor este número más tardará el robot, recuerda 1 segundo por cada mil escrito en el valor.
+Son milisegundos (2mil milisegundos = 2 segundos)</t>
+  </si>
+  <si>
+    <t>DarFormatoReporte</t>
+  </si>
+  <si>
+    <t>ActivarModoDebug</t>
+  </si>
+  <si>
+    <t>Si el Value es TRUE solo realizará un recorrido a las 2 primeras clases que encuentre. La intención de esta bandera es agilizar la depuración.
+Si el Value es False, realizará el recorrido de todas las clases que encuentre.</t>
+  </si>
+  <si>
+    <t>Si deseas no dar formato (tamaño de columnas, añadir comentarios) para agilizar el resultado, puedes cambiar esta bandera a FALSE.</t>
+  </si>
+  <si>
+    <t>Navegador</t>
+  </si>
+  <si>
+    <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
   <si>
     <t>Si desea realizar una nueva revisión proporcione la url del curso que desea revisar.
 Puedes añadir múltiples urls concatenando con un ; 
 Ejemplo: https://platzi.com/clases/diseno-interfaz/ ; platzi.com/uipath
-Si dejas vacio este campo, se leerá el archivo previamente geneardo.</t>
-  </si>
-  <si>
-    <t>URLCursos</t>
-  </si>
-  <si>
-    <t>RutaPadre</t>
-  </si>
-  <si>
-    <t>NombreReporte</t>
-  </si>
-  <si>
-    <t>Comentarios.xlsx</t>
-  </si>
-  <si>
-    <t>Nombre que se le asignará al archivo excel del reporte final.</t>
-  </si>
-  <si>
-    <t>Ruta donde se guardará el archivo final, capturas de pantalla y logs.</t>
-  </si>
-  <si>
-    <t>LogLocal</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>True: generará un log llamadlo log.txt en la ruta padre.
-False: No generará ningún reporte.</t>
-  </si>
-  <si>
-    <t>varTimeOutGeneral</t>
-  </si>
-  <si>
-    <t>ExtraerRespuestasDeComentarios</t>
-  </si>
-  <si>
-    <t>SeguimientoManual</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>SeguimientoAutomático</t>
-  </si>
-  <si>
-    <t>Volverá el robot un robot Atendido y solicitará respuesta para cada comentario encontrado.</t>
-  </si>
-  <si>
-    <t>Responderá automáticamente a cada comentario que cumpla las condiciones de respuesta automática</t>
-  </si>
-  <si>
-    <t>Indica si deseas o no extraer las respuestas de cada comentario.</t>
-  </si>
-  <si>
-    <t>delayGenerarReporte</t>
-  </si>
-  <si>
-    <t>Este valor se convierte en Segundos, al colocar 1 genera que cada actividad de formato tenga un tiempo de espera de &lt;tuvalor&gt;*2 segundo. Son apróximadamente 15 actividades de Formato.</t>
-  </si>
-  <si>
-    <t>Entre mayor este número más tardará el robot, recuerda 1 segundo por cada mil escrito en el valor.
-Son milisegundos (2mil milisegundos = 2 segundos)</t>
+Si dejas vacio este campo, se leerá el archivo previamente geneardo.
+https://platzi.com/clases/uipath/</t>
   </si>
   <si>
     <t>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</t>
-  </si>
-  <si>
-    <t>DarFormatoReporte</t>
-  </si>
-  <si>
-    <t>ActivarModoDebug</t>
-  </si>
-  <si>
-    <t>Si el Value es TRUE solo realizará un recorrido a las 2 primeras clases que encuentre. La intención de esta bandera es agilizar la depuración.
-Si el Value es False, realizará el recorrido de todas las clases que encuentre.</t>
-  </si>
-  <si>
-    <t>Si deseas no dar formato (tamaño de columnas, añadir comentarios) para agilizar el resultado, puedes cambiar esta bandera a FALSE.</t>
-  </si>
-  <si>
-    <t>https://platzi.com/clases/uipath/</t>
-  </si>
-  <si>
-    <t>Navegador</t>
-  </si>
-  <si>
-    <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).</t>
-  </si>
-  <si>
-    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -614,7 +612,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -682,135 +680,137 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="60">
+    <row r="4" spans="1:26" ht="75">
       <c r="A4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>56</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="9" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="60">
       <c r="A5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="45">
       <c r="A7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="6">
         <v>2000</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30">
       <c r="A8" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="30">
       <c r="A10" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="30">
       <c r="A11" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="30">
       <c r="A12" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="45">
       <c r="A13" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="30">
       <c r="A14" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <phoneticPr fontId="2"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Valor inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B14" xr:uid="{D5ABB2E3-00BB-47FB-BB5C-0A9FF1640B9C}">
       <formula1>"Firefox, Edge, Chrome, InternetExplorer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B13 B12 B10 B8 B9" xr:uid="{128881F2-0E38-4DFD-A3D4-6EB6C88D1173}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B12:B13 B8:B10" xr:uid="{128881F2-0E38-4DFD-A3D4-6EB6C88D1173}">
       <formula1>"True, False"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Error:" error="No puede ser vacío, o el robot no funcionará." promptTitle="El campo: Ruta Padre" prompt="No puede ser vacío, o el robot no funcionará." sqref="B5" xr:uid="{14A6CD44-8F41-4529-A27D-9872A464FFA8}">
+      <formula1>ISBLANK($B$5)=FALSE</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,13 +948,13 @@
     </row>
     <row r="9" spans="1:26" ht="30">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Control de error cuando no puede leer el nombre del curso. Corrección de selector para dar clic en "ir a curso" Merge del archivo "takescreenshot" que estaba en 2 carpetas distintas.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C719AB-BA20-47F3-A280-4DF756DAE073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E2853092-58FE-45BF-BD7C-F1F178AED29B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E1E69965-BDDE-428B-BA85-D3A3BF8824A5}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -207,16 +207,18 @@
   </si>
   <si>
     <t>Firefox</t>
+  </si>
+  <si>
+    <t>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</t>
   </si>
   <si>
     <t>Si desea realizar una nueva revisión proporcione la url del curso que desea revisar.
 Puedes añadir múltiples urls concatenando con un ; 
 Ejemplo: https://platzi.com/clases/diseno-interfaz/ ; platzi.com/uipath
-Si dejas vacio este campo, se leerá el archivo previamente geneardo.
-https://platzi.com/clases/uipath/</t>
-  </si>
-  <si>
-    <t>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</t>
+Si dejas vacio este campo, se leerá el archivo previamente geneardo.</t>
+  </si>
+  <si>
+    <t>platzi.com/uipath</t>
   </si>
 </sst>
 </file>
@@ -612,7 +614,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -680,13 +682,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="75">
+    <row r="4" spans="1:26" ht="60">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="60">
@@ -694,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>35</v>
@@ -738,7 +742,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>44</v>
@@ -749,7 +753,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Se corrige un bug que colocaba // a la ruta del reporte.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E2853092-58FE-45BF-BD7C-F1F178AED29B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E1E69965-BDDE-428B-BA85-D3A3BF8824A5}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C70BA99-3300-4BDF-A099-C76CC70B48F7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33270" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,6 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -209,9 +201,6 @@
     <t>Firefox</t>
   </si>
   <si>
-    <t>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</t>
-  </si>
-  <si>
     <t>Si desea realizar una nueva revisión proporcione la url del curso que desea revisar.
 Puedes añadir múltiples urls concatenando con un ; 
 Ejemplo: https://platzi.com/clases/diseno-interfaz/ ; platzi.com/uipath
@@ -219,6 +208,9 @@
   </si>
   <si>
     <t>platzi.com/uipath</t>
+  </si>
+  <si>
+    <t>E:\Archivos\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -613,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -687,18 +679,18 @@
         <v>30</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="60">
+    <row r="5" spans="1:26">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>35</v>
@@ -785,7 +777,7 @@
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -889,7 +881,7 @@
       </c>
       <c r="B3" t="str">
         <f>Settings!B5</f>
-        <v>E:\Archivos\OneDrive\Programación\GitHub\UitPath\FindComments_PlatziCourse\Data\Output</v>
+        <v>E:\Archivos\Downloads\</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Actualización de Config (descripción) y Readme.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C70BA99-3300-4BDF-A099-C76CC70B48F7}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56E8336B-84C6-4F11-84EA-1D20A37E7E87}"/>
   <bookViews>
-    <workbookView xWindow="33270" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,10 +87,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -129,9 +125,6 @@
     <t>Comentarios.xlsx</t>
   </si>
   <si>
-    <t>Nombre que se le asignará al archivo excel del reporte final.</t>
-  </si>
-  <si>
     <t>Ruta donde se guardará el archivo final, capturas de pantalla y logs.</t>
   </si>
   <si>
@@ -160,64 +153,109 @@
     <t>SeguimientoAutomático</t>
   </si>
   <si>
-    <t>Volverá el robot un robot Atendido y solicitará respuesta para cada comentario encontrado.</t>
-  </si>
-  <si>
-    <t>Responderá automáticamente a cada comentario que cumpla las condiciones de respuesta automática</t>
-  </si>
-  <si>
-    <t>Indica si deseas o no extraer las respuestas de cada comentario.</t>
-  </si>
-  <si>
     <t>delayGenerarReporte</t>
   </si>
   <si>
-    <t>Este valor se convierte en Segundos, al colocar 1 genera que cada actividad de formato tenga un tiempo de espera de &lt;tuvalor&gt;*2 segundo. Son apróximadamente 15 actividades de Formato.</t>
+    <t>DarFormatoReporte</t>
+  </si>
+  <si>
+    <t>ActivarModoDebug</t>
+  </si>
+  <si>
+    <t>Navegador</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>platzi.com/uipath</t>
+  </si>
+  <si>
+    <t>E:\Archivos\Downloads\</t>
   </si>
   <si>
     <t>Entre mayor este número más tardará el robot, recuerda 1 segundo por cada mil escrito en el valor.
-Son milisegundos (2mil milisegundos = 2 segundos)</t>
-  </si>
-  <si>
-    <t>DarFormatoReporte</t>
-  </si>
-  <si>
-    <t>ActivarModoDebug</t>
-  </si>
-  <si>
-    <t>Si el Value es TRUE solo realizará un recorrido a las 2 primeras clases que encuentre. La intención de esta bandera es agilizar la depuración.
-Si el Value es False, realizará el recorrido de todas las clases que encuentre.</t>
-  </si>
-  <si>
-    <t>Si deseas no dar formato (tamaño de columnas, añadir comentarios) para agilizar el resultado, puedes cambiar esta bandera a FALSE.</t>
-  </si>
-  <si>
-    <t>Navegador</t>
-  </si>
-  <si>
-    <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).</t>
-  </si>
-  <si>
-    <t>Firefox</t>
+Son milisegundos (2mil milisegundos = 2 segundos)
+Tiempo estimado : 
+Puede aumentar el tiempo de ejecución del robot en los segundos indicados multiplicado por 50 acciones, es un apróximado debido a que es una mezcla entre ese tiempo de espera y la velocidad de tu Internet para mostrar las páginas web.</t>
+  </si>
+  <si>
+    <t>Indica si deseas o no extraer las respuestas de cada comentario.
+Tiempo estimado :
+Apróximadamente 6 minutos extras de duración cada 200 comentarios.</t>
+  </si>
+  <si>
+    <t>Volverá el robot un robot Atendido y solicitará respuesta para cada comentario encontrado.
+Tiempo estimado :
+Tiempo extra indefinido, ya qué requiere interacción humana (se vuelve un robot asistido).</t>
+  </si>
+  <si>
+    <t>Responderá automáticamente a cada comentario que cumpla las condiciones de respuesta automática
+Tiempo estimado :
+Apróximadamente 5 minutos cada 100 comentarios respondidos o "marcados con corazón" por este Módulo.</t>
+  </si>
+  <si>
+    <t>Este valor se convierte en Segundos, al colocar 1 genera que cada actividad de formato tenga un tiempo de espera de &lt;tuvalor&gt;*2 segundos. Son apróximadamente 15 actividades de Formato.</t>
+  </si>
+  <si>
+    <t>Si deseas no dar formato (tamaño de columnas, añadir comentarios) para agilizar el resultado, puedes cambiar esta bandera a FALSE.
+Tiempo estimado :
+Incrementa el tiempo de ejecución en 3 minutos para dar formato al documento.</t>
+  </si>
+  <si>
+    <t>Si el Value es TRUE solo realizará un recorrido a las 3 primeras clases que encuentre. La intención de esta bandera es agilizar la depuración.
+Si el Value es False, realizará el recorrido de todas las clases que encuentre.
+Tiempo estimado :
+Reduce el tiempo un 90% por curso.</t>
+  </si>
+  <si>
+    <t>Indicar el tipo de navegador que utilizará el robot para extraer los datos, recuerda que este navegador debe tener instalao el Plugin de UiPath (excepto para Iexplorer).
+Si este campo llega a estar vacío, se usará Firefox como navegador por defecto (y si no lo tienes instalado, causará fallas en la ejecución del robot.</t>
+  </si>
+  <si>
+    <t>Nombre de la cola de Orquestador, no es utilizado, se deja por buenas prácticas.</t>
   </si>
   <si>
     <t>Si desea realizar una nueva revisión proporcione la url del curso que desea revisar.
 Puedes añadir múltiples urls concatenando con un ; 
 Ejemplo: https://platzi.com/clases/diseno-interfaz/ ; platzi.com/uipath
-Si dejas vacio este campo, se leerá el archivo previamente geneardo.</t>
-  </si>
-  <si>
-    <t>platzi.com/uipath</t>
-  </si>
-  <si>
-    <t>E:\Archivos\Downloads\</t>
+Si dejas vacio este campo, se leerá el archivo previamente geneardo.
+Tiempo estimado :
+Un promedio de 7 minutos por Curso (de 40 clases) sin los módulos indicados abajo (los true o false).
+Si se deja vacío se reduce el tiempo un 95% bajando a 1 minuto. (No navega a ningun sitio web a extraer datos).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nombre que se le asignará al archivo excel del reporte final.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Importante</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>: si se omite o utiliza una extensión distinta a ".xlsx" el archivo generado no tendrá extensión y puede fallar la generación del reporte.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -241,13 +279,40 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -262,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -288,6 +353,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -654,159 +732,148 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="135">
+      <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>21</v>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30">
-      <c r="A3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
+    <row r="4" spans="1:26">
+      <c r="A4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="60">
-      <c r="A4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>57</v>
+    <row r="5" spans="1:26" ht="45">
+      <c r="A5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
-      <c r="A5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="100.5" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2000</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="45">
       <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="45">
+      <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="6">
-        <v>2000</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>49</v>
+      <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30">
-      <c r="A8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="75">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="30">
       <c r="A10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="60">
+      <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="75">
+      <c r="A12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="60">
+      <c r="A13" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="30">
-      <c r="A11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="30">
-      <c r="A12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="45">
-      <c r="A13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="30">
-      <c r="A14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="B13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="2"/>
   <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Valor inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B14" xr:uid="{D5ABB2E3-00BB-47FB-BB5C-0A9FF1640B9C}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Valor inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B13" xr:uid="{D5ABB2E3-00BB-47FB-BB5C-0A9FF1640B9C}">
       <formula1>"Firefox, Edge, Chrome, InternetExplorer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B12:B13 B8:B10" xr:uid="{128881F2-0E38-4DFD-A3D4-6EB6C88D1173}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Valor Inválido" error="Colocar un valor fuera de la lista puede causar un error en el Robot ya que este solo tiene soporte en código a los valores indicados." sqref="B11:B12 B7:B9" xr:uid="{128881F2-0E38-4DFD-A3D4-6EB6C88D1173}">
       <formula1>"True, False"</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Error:" error="No puede ser vacío, o el robot no funcionará." promptTitle="El campo: Ruta Padre" prompt="No puede ser vacío, o el robot no funcionará." sqref="B5" xr:uid="{14A6CD44-8F41-4529-A27D-9872A464FFA8}">
-      <formula1>ISBLANK($B$5)=FALSE</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Error:" error="No puede ser vacío, o el robot no funcionará." promptTitle="El campo: Ruta Padre" prompt="No puede ser vacío, o el robot no funcionará." sqref="B4" xr:uid="{14A6CD44-8F41-4529-A27D-9872A464FFA8}">
+      <formula1>ISBLANK($B$4)=FALSE</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -819,7 +886,7 @@
   <dimension ref="A1:Z985"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -872,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -880,7 +947,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="str">
-        <f>Settings!B5</f>
+        <f>Settings!B4</f>
         <v>E:\Archivos\Downloads\</v>
       </c>
       <c r="C3" t="s">
@@ -895,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -917,7 +984,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -928,7 +995,7 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -939,21 +1006,31 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Se corrige filtro de repetidos, estaba borrando todo en vez de dejar los valores únicos.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56E8336B-84C6-4F11-84EA-1D20A37E7E87}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FBEF3E7-6A22-4154-A2A8-8D8F4CD90CEE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29235" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Se actualizan Dependencias a 2020.8 Se corrige obtención de URL, ya qué se modificó la estructura html del sitio web.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FBEF3E7-6A22-4154-A2A8-8D8F4CD90CEE}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5631ADBE-DEB2-40AB-870C-61C8986BA379}"/>
   <bookViews>
-    <workbookView xWindow="29235" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Actualización de versión y file config path (esto para uso personal)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse_UiPath/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5631ADBE-DEB2-40AB-870C-61C8986BA379}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7590" yWindow="1485" windowWidth="21570" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -683,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualización de DLL's/Dependencias Se optimiza el código para adaptarse a los cambios de UI de Platzi.com
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56c8892e474b3fb5/Programación/GitHub/UitPath/FindComments_PlatziCourse_UiPath/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5631ADBE-DEB2-40AB-870C-61C8986BA379}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{AE9A424F-E6E6-457B-860A-49D736296E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7DD190DE-06FA-42C7-9DB3-C9E7D2D259CF}"/>
   <bookViews>
-    <workbookView xWindow="7590" yWindow="1485" windowWidth="21570" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Firefox</t>
-  </si>
-  <si>
-    <t>platzi.com/uipath</t>
   </si>
   <si>
     <t>E:\Archivos\Downloads\</t>
@@ -249,6 +246,9 @@
       </rPr>
       <t>: si se omite o utiliza una extensión distinta a ".xlsx" el archivo generado no tendrá extensión y puede fallar la generación del reporte.</t>
     </r>
+  </si>
+  <si>
+    <t>platzi.com/uipath;https://platzi.com/clases/analista-rpa/</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -738,7 +738,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="135">
@@ -746,10 +746,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -757,7 +757,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>33</v>
@@ -771,7 +771,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="100.5" customHeight="1">
@@ -782,7 +782,7 @@
         <v>2000</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="45">
@@ -793,7 +793,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="45">
@@ -804,7 +804,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="75">
@@ -815,7 +815,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="30">
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="60">
@@ -837,7 +837,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="75">
@@ -848,7 +848,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="60">
@@ -859,7 +859,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>